<commit_message>
* ParentId: TRE-95 (OR-550-BE) (1) - Fix branch revenue Task Id: TRE-95 (OR-550-BE) Type: Development Description: - Fix branch revenue
</commit_message>
<xml_diff>
--- a/app/order-api/public/templates/excel/export-revenue.xlsx
+++ b/app/order-api/public/templates/excel/export-revenue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Order\order\app\order-api\public\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9597C770-297A-427B-9FB3-C38F12145307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB7FEED-7F25-48BB-A2F6-606E76B32491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="13176" xr2:uid="{59E5C100-1BA5-42F9-BF8C-49F5B3F156A4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{59E5C100-1BA5-42F9-BF8C-49F5B3F156A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>BÁO CÁO DOANH THU</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Tổng doanh thu ví nội bộ</t>
+  </si>
+  <si>
+    <t>Tổng giảm giá đơn dưới 2.000đ</t>
   </si>
 </sst>
 </file>
@@ -509,28 +512,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5DBBB0D-6011-49B5-900C-FA0A48448A03}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="19.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="14.33203125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="19.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" style="1" customWidth="1"/>
+    <col min="6" max="7" width="16.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="43.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" ht="43.2" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -544,43 +547,44 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -600,29 +604,32 @@
         <v>7</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A1:L1"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>

<commit_message>
* Parent ID: VC-550-BE (3) Task Id: VC-550-BE Type: Development Description: + Fix branch revenue
</commit_message>
<xml_diff>
--- a/app/order-api/public/templates/excel/export-revenue.xlsx
+++ b/app/order-api/public/templates/excel/export-revenue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Order\order\app\order-api\public\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB7FEED-7F25-48BB-A2F6-606E76B32491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114D4AD8-6BFB-460B-B3AD-1F5C38AE280D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{59E5C100-1BA5-42F9-BF8C-49F5B3F156A4}"/>
   </bookViews>
@@ -50,9 +50,6 @@
     <t>STT</t>
   </si>
   <si>
-    <t>Ngày</t>
-  </si>
-  <si>
     <t>Chi nhánh</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>Tổng giảm giá đơn dưới 2.000đ</t>
+  </si>
+  <si>
+    <t>Thời gian</t>
   </si>
 </sst>
 </file>
@@ -172,11 +172,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -515,7 +515,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -534,92 +534,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="43.2" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
     </row>
     <row r="8" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* ParentId: VC-550-BE (5) Task Id: VC-550-BE Type: Development Description: - Add point method for branch revenue
</commit_message>
<xml_diff>
--- a/app/order-api/public/templates/excel/export-revenue.xlsx
+++ b/app/order-api/public/templates/excel/export-revenue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Order\order\app\order-api\public\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114D4AD8-6BFB-460B-B3AD-1F5C38AE280D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31015B38-BE6F-4634-9FAD-6AB7E8C26168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{59E5C100-1BA5-42F9-BF8C-49F5B3F156A4}"/>
   </bookViews>
@@ -59,9 +59,6 @@
     <t>Tổng giảm giá</t>
   </si>
   <si>
-    <t>Tổng xu</t>
-  </si>
-  <si>
     <t>Ngày xuất</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>Thời gian</t>
+  </si>
+  <si>
+    <t>Tổng doanh thu xu</t>
   </si>
 </sst>
 </file>
@@ -515,7 +515,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -558,7 +558,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -579,7 +579,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -589,13 +589,13 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>5</v>
@@ -604,22 +604,22 @@
         <v>6</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* ParentId: TRE-210-BE (1) Task Id: TRE-210-BE Type: Development Description: - Implement accumulated points: order, invoice, temporary invoice, branch revenue - Add percent accumulated point to system config service
</commit_message>
<xml_diff>
--- a/app/order-api/public/templates/excel/export-revenue.xlsx
+++ b/app/order-api/public/templates/excel/export-revenue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Order\order\app\order-api\public\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31015B38-BE6F-4634-9FAD-6AB7E8C26168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6513B6B-027D-425F-8717-811A5D161ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{59E5C100-1BA5-42F9-BF8C-49F5B3F156A4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{59E5C100-1BA5-42F9-BF8C-49F5B3F156A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>BÁO CÁO DOANH THU</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Tổng doanh thu xu</t>
+  </si>
+  <si>
+    <t>Tổng điểm tích lũy</t>
   </si>
 </sst>
 </file>
@@ -512,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5DBBB0D-6011-49B5-900C-FA0A48448A03}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,16 +527,16 @@
     <col min="2" max="3" width="19.5546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.88671875" style="1" customWidth="1"/>
-    <col min="6" max="7" width="16.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="19.109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="1"/>
+    <col min="6" max="8" width="16.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="18.33203125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="43.2" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:13" ht="43.2" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -548,43 +551,44 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
     </row>
-    <row r="8" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -607,24 +611,27 @@
         <v>15</v>
       </c>
       <c r="H8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:M1"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>

</xml_diff>

<commit_message>
* ParentId: TRE-219-BE (2) Task Id: TRE-219-BE Type: Development Description: - Add credit card for branch revenue, export excel, pdf
</commit_message>
<xml_diff>
--- a/app/order-api/public/templates/excel/export-revenue.xlsx
+++ b/app/order-api/public/templates/excel/export-revenue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Order\order\app\order-api\public\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6513B6B-027D-425F-8717-811A5D161ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970CB749-95D5-4D00-A8ED-F86AFF6CFE0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{59E5C100-1BA5-42F9-BF8C-49F5B3F156A4}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="27264" windowHeight="12660" xr2:uid="{59E5C100-1BA5-42F9-BF8C-49F5B3F156A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>BÁO CÁO DOANH THU</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Tổng điểm tích lũy</t>
+  </si>
+  <si>
+    <t>Tổng doanh thu quẹt thẻ</t>
   </si>
 </sst>
 </file>
@@ -515,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5DBBB0D-6011-49B5-900C-FA0A48448A03}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,10 +536,11 @@
     <col min="11" max="11" width="16.6640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="18.6640625" style="1" customWidth="1"/>
     <col min="13" max="13" width="18.33203125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="1"/>
+    <col min="14" max="14" width="20.88671875" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="43.2" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:14" ht="43.2" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -553,42 +557,42 @@
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
     </row>
-    <row r="8" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -627,6 +631,9 @@
       </c>
       <c r="M8" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* ParentId: TRE-233-BE (7) Task Id: TRE-233-BE Type: Development Description: - Add delivery fee for branch revenue
</commit_message>
<xml_diff>
--- a/app/order-api/public/templates/excel/export-revenue.xlsx
+++ b/app/order-api/public/templates/excel/export-revenue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Order\order\app\order-api\public\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970CB749-95D5-4D00-A8ED-F86AFF6CFE0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F22952-F4F4-4152-99B9-C0E73AD074AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="27264" windowHeight="12660" xr2:uid="{59E5C100-1BA5-42F9-BF8C-49F5B3F156A4}"/>
+    <workbookView xWindow="1272" yWindow="2244" windowWidth="29364" windowHeight="12660" xr2:uid="{59E5C100-1BA5-42F9-BF8C-49F5B3F156A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>BÁO CÁO DOANH THU</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Tổng doanh thu quẹt thẻ</t>
+  </si>
+  <si>
+    <t>Tổng phí giao hàng</t>
   </si>
 </sst>
 </file>
@@ -518,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5DBBB0D-6011-49B5-900C-FA0A48448A03}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,10 +540,11 @@
     <col min="12" max="12" width="18.6640625" style="1" customWidth="1"/>
     <col min="13" max="13" width="18.33203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="20.88671875" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="1"/>
+    <col min="15" max="15" width="18.77734375" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="43.2" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:15" ht="43.2" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -557,42 +561,42 @@
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
     </row>
-    <row r="8" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -634,6 +638,9 @@
       </c>
       <c r="N8" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* ParentId: TRE-222-BE (4) Task Id: TRE-222-BE Type: Development Description: - Fix branch revenue have cost of gift product
</commit_message>
<xml_diff>
--- a/app/order-api/public/templates/excel/export-revenue.xlsx
+++ b/app/order-api/public/templates/excel/export-revenue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Order\order\app\order-api\public\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F22952-F4F4-4152-99B9-C0E73AD074AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009D8B70-4837-4129-AB2C-6561795A4ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1272" yWindow="2244" windowWidth="29364" windowHeight="12660" xr2:uid="{59E5C100-1BA5-42F9-BF8C-49F5B3F156A4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{59E5C100-1BA5-42F9-BF8C-49F5B3F156A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>BÁO CÁO DOANH THU</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Tổng phí giao hàng</t>
+  </si>
+  <si>
+    <t>Tổng tiền quà tặng</t>
   </si>
 </sst>
 </file>
@@ -521,30 +524,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5DBBB0D-6011-49B5-900C-FA0A48448A03}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.33203125" style="1" customWidth="1"/>
     <col min="2" max="3" width="19.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" style="1" customWidth="1"/>
-    <col min="6" max="8" width="16.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="18.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="20.88671875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="18.77734375" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="5" width="16.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" style="1" customWidth="1"/>
+    <col min="7" max="9" width="16.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19.109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="20.88671875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="18.77734375" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="43.2" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:16" ht="43.2" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -560,43 +563,44 @@
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
     </row>
-    <row r="8" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -610,42 +614,45 @@
         <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="N8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="P8" s="2" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A1:N1"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>

</xml_diff>